<commit_message>
bieu do trinh tu
</commit_message>
<xml_diff>
--- a/Documents/Biểu đồ Gantt công việc.xlsx
+++ b/Documents/Biểu đồ Gantt công việc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bài trên lớp\New folder\New folder\PTTKPM25-26_CLASSN05_NHOM7\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84C7DAA1-52CF-4414-A23F-50C632EE24B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DD7C8E-4DBE-472F-ABD3-DE429D10A1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4B9EB8C9-4F0A-4E4B-B2B3-51533343E813}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>STT</t>
   </si>
@@ -86,15 +86,31 @@
     <t xml:space="preserve"> Thiết kế Lớp và Tạo cơ sở code</t>
   </si>
   <si>
-    <t>Hoàn, Hiếu, An</t>
-  </si>
-  <si>
-    <t>An, Ninh</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Xác định lớp đối tượng chính
  Vẽ Class Diagram
 Tạo file Java với skeleton code cho các lớp</t>
+  </si>
+  <si>
+    <t>Vẽ Biểu đồ Trình tự</t>
+  </si>
+  <si>
+    <t>An</t>
+  </si>
+  <si>
+    <t>Hoàn, An</t>
+  </si>
+  <si>
+    <t>Vẽ Biểu đồ Trình tự (Sequence Diagram) để thể hiện luồng thông
+điệp giữa các đối tượng</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện</t>
+  </si>
+  <si>
+    <t>Ninh</t>
+  </si>
+  <si>
+    <t>Phác thảo giao diện cho chức năng</t>
   </si>
 </sst>
 </file>
@@ -153,16 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -180,13 +190,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -219,8 +234,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>236520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Viết tay 4">
@@ -239,7 +254,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="5" name="Viết tay 4">
@@ -284,8 +299,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>213540</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="10" name="Viết tay 9">
@@ -304,7 +319,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="10" name="Viết tay 9">
@@ -349,8 +364,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>274500</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="20" name="Viết tay 19">
@@ -369,7 +384,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="20" name="Viết tay 19">
@@ -409,13 +424,13 @@
       <xdr:rowOff>258540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>259260</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="21" name="Viết tay 20">
@@ -429,12 +444,142 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10668000" y="2376900"/>
-            <a:ext cx="480060" cy="720"/>
+            <a:off x="11071860" y="2376900"/>
+            <a:ext cx="670560" cy="720"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="21" name="Viết tay 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF04616E-160F-497D-99CA-29FA6194C834}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10578034" y="2017620"/>
+              <a:ext cx="659633" cy="720000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>258540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>259260</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="4" name="Viết tay 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{986F5AC3-0920-404F-9FC5-9D24819016CE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11399520" y="2879820"/>
+            <a:ext cx="967740" cy="720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="21" name="Viết tay 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF04616E-160F-497D-99CA-29FA6194C834}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10578034" y="2017620"/>
+              <a:ext cx="659633" cy="720000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>556260</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>281400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>754380</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>282120</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Viết tay 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EB0135C-2393-4204-A5FE-BA4979573BCE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11422380" y="3405600"/>
+            <a:ext cx="967740" cy="720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="21" name="Viết tay 20">
@@ -587,7 +732,69 @@
       <inkml:brushProperty name="ignorePressure" value="1"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 0,'1333'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 0,'1862'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-09-18T01:41:24.238"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.5" units="cm"/>
+      <inkml:brushProperty name="height" value="1" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFC00"/>
+      <inkml:brushProperty name="tip" value="rectangle"/>
+      <inkml:brushProperty name="rasterOp" value="maskPen"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 0,'2687'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-09-18T01:43:31.364"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.5" units="cm"/>
+      <inkml:brushProperty name="height" value="1" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFFC00"/>
+      <inkml:brushProperty name="tip" value="rectangle"/>
+      <inkml:brushProperty name="rasterOp" value="maskPen"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 0,'2687'0'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -911,7 +1118,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="39.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -924,37 +1131,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8"/>
       <c r="F2" s="1">
         <v>18</v>
       </c>
@@ -978,192 +1185,203 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="11"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="11"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="11"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="11"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="11"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:12" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="11"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="11"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="11"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="12"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="12"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="12"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="12"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:5" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="12"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="H1:L1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>